<commit_message>
follow soem_advr commit, not use getSDO_byname, add coman_test
</commit_message>
<xml_diff>
--- a/configs/Disney Coman motor parameters.xlsx
+++ b/configs/Disney Coman motor parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="15195" windowHeight="10485"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="15195" windowHeight="10485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Legs" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="90">
   <si>
     <t>Joint number</t>
   </si>
@@ -277,6 +277,15 @@
   </si>
   <si>
     <t>Cal pos</t>
+  </si>
+  <si>
+    <t>Pos Integral Limit</t>
+  </si>
+  <si>
+    <t>Torque Integral Limit</t>
+  </si>
+  <si>
+    <t>100k</t>
   </si>
 </sst>
 </file>
@@ -382,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -455,6 +464,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,10 +765,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:R36"/>
+  <dimension ref="A3:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -862,7 +874,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="8">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>23</v>
@@ -884,8 +896,7 @@
         <v>50</v>
       </c>
       <c r="J8" s="21">
-        <f>I8 * 200000 * 3.14159 / (360 * 100000)</f>
-        <v>0.87266388888888891</v>
+        <v>0.85</v>
       </c>
       <c r="K8" s="20">
         <v>81920</v>
@@ -896,7 +907,9 @@
       <c r="M8" s="5">
         <v>11693</v>
       </c>
-      <c r="N8" s="5"/>
+      <c r="N8" s="5">
+        <v>1455116</v>
+      </c>
       <c r="O8" s="11" t="s">
         <v>27</v>
       </c>
@@ -914,7 +927,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="8" t="s">
@@ -927,15 +940,13 @@
         <v>-30</v>
       </c>
       <c r="H9" s="21">
-        <f t="shared" ref="H9:H21" si="0">G9 * 200000 * 3.14159 / (360 * 100000)</f>
-        <v>-0.52359833333333339</v>
+        <v>-0.5</v>
       </c>
       <c r="I9" s="5">
         <v>30</v>
       </c>
       <c r="J9" s="21">
-        <f t="shared" ref="J9:J21" si="1">I9 * 200000 * 3.14159 / (360 * 100000)</f>
-        <v>0.52359833333333339</v>
+        <v>0.5</v>
       </c>
       <c r="K9" s="20">
         <v>8192</v>
@@ -944,9 +955,11 @@
         <v>0</v>
       </c>
       <c r="M9" s="5">
-        <v>5346</v>
-      </c>
-      <c r="N9" s="5"/>
+        <v>5342</v>
+      </c>
+      <c r="N9" s="5">
+        <v>1065189</v>
+      </c>
       <c r="O9" s="11" t="s">
         <v>26</v>
       </c>
@@ -964,7 +977,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>23</v>
@@ -979,14 +992,14 @@
         <v>-110</v>
       </c>
       <c r="H10" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H10:H21" si="0">G10 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>-1.9198605555555555</v>
       </c>
       <c r="I10" s="5">
         <v>45</v>
       </c>
       <c r="J10" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J10:J21" si="1">I10 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>0.78539749999999997</v>
       </c>
       <c r="K10" s="20">
@@ -998,7 +1011,9 @@
       <c r="M10" s="5">
         <v>8430</v>
       </c>
-      <c r="N10" s="5"/>
+      <c r="N10" s="5">
+        <v>3503108</v>
+      </c>
       <c r="O10" s="11" t="s">
         <v>27</v>
       </c>
@@ -1016,7 +1031,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="8">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>23</v>
@@ -1031,8 +1046,7 @@
         <v>-110</v>
       </c>
       <c r="H11" s="21">
-        <f t="shared" si="0"/>
-        <v>-1.9198605555555555</v>
+        <v>-1.9</v>
       </c>
       <c r="I11" s="5">
         <v>45</v>
@@ -1048,9 +1062,11 @@
         <v>3000</v>
       </c>
       <c r="M11" s="5">
-        <v>9625</v>
-      </c>
-      <c r="N11" s="5"/>
+        <v>9626</v>
+      </c>
+      <c r="N11" s="5">
+        <v>3477214</v>
+      </c>
       <c r="O11" s="11" t="s">
         <v>26</v>
       </c>
@@ -1068,7 +1084,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="8">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="8" t="s">
@@ -1081,8 +1097,7 @@
         <v>-60</v>
       </c>
       <c r="H12" s="21">
-        <f t="shared" si="0"/>
-        <v>-1.0471966666666668</v>
+        <v>-1</v>
       </c>
       <c r="I12" s="5">
         <v>25</v>
@@ -1100,7 +1115,9 @@
       <c r="M12" s="5">
         <v>7394</v>
       </c>
-      <c r="N12" s="5"/>
+      <c r="N12" s="5">
+        <v>1130379</v>
+      </c>
       <c r="O12" s="11" t="s">
         <v>26</v>
       </c>
@@ -1118,7 +1135,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="8">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="8" t="s">
@@ -1138,8 +1155,7 @@
         <v>50</v>
       </c>
       <c r="J13" s="21">
-        <f t="shared" si="1"/>
-        <v>0.87266388888888891</v>
+        <v>0.86</v>
       </c>
       <c r="K13" s="20">
         <v>8192</v>
@@ -1150,7 +1166,9 @@
       <c r="M13" s="5">
         <v>4894</v>
       </c>
-      <c r="N13" s="5"/>
+      <c r="N13" s="5">
+        <v>1113782</v>
+      </c>
       <c r="O13" s="11" t="s">
         <v>27</v>
       </c>
@@ -1168,7 +1186,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="8">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>23</v>
@@ -1190,8 +1208,7 @@
         <v>110</v>
       </c>
       <c r="J14" s="21">
-        <f t="shared" si="1"/>
-        <v>1.9198605555555555</v>
+        <v>1.88</v>
       </c>
       <c r="K14" s="20">
         <v>81920</v>
@@ -1202,7 +1219,9 @@
       <c r="M14" s="5">
         <v>8413</v>
       </c>
-      <c r="N14" s="5"/>
+      <c r="N14" s="5">
+        <v>1227551</v>
+      </c>
       <c r="O14" s="11" t="s">
         <v>27</v>
       </c>
@@ -1220,7 +1239,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="8">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>23</v>
@@ -1235,8 +1254,7 @@
         <v>-70</v>
       </c>
       <c r="H15" s="21">
-        <f t="shared" si="0"/>
-        <v>-1.2217294444444444</v>
+        <v>-1.2</v>
       </c>
       <c r="I15" s="5">
         <v>50</v>
@@ -1252,9 +1270,11 @@
         <v>8000</v>
       </c>
       <c r="M15" s="5">
-        <v>7920</v>
-      </c>
-      <c r="N15" s="5"/>
+        <v>7924</v>
+      </c>
+      <c r="N15" s="5">
+        <v>1156455</v>
+      </c>
       <c r="O15" s="11" t="s">
         <v>27</v>
       </c>
@@ -1272,7 +1292,7 @@
         <v>10</v>
       </c>
       <c r="C16" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="8" t="s">
@@ -1302,9 +1322,11 @@
         <v>4000</v>
       </c>
       <c r="M16" s="5">
-        <v>9001</v>
-      </c>
-      <c r="N16" s="5"/>
+        <v>8949</v>
+      </c>
+      <c r="N16" s="5">
+        <v>1079648</v>
+      </c>
       <c r="O16" s="11" t="s">
         <v>26</v>
       </c>
@@ -1322,7 +1344,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="8">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="8" t="s">
@@ -1335,15 +1357,13 @@
         <v>-25</v>
       </c>
       <c r="H17" s="21">
-        <f t="shared" si="0"/>
-        <v>-0.43633194444444445</v>
+        <v>-0.4</v>
       </c>
       <c r="I17" s="5">
         <v>60</v>
       </c>
       <c r="J17" s="21">
-        <f t="shared" si="1"/>
-        <v>1.0471966666666668</v>
+        <v>1</v>
       </c>
       <c r="K17" s="20">
         <v>8192</v>
@@ -1354,7 +1374,9 @@
       <c r="M17" s="5">
         <v>1189</v>
       </c>
-      <c r="N17" s="5"/>
+      <c r="N17" s="5">
+        <v>1052151</v>
+      </c>
       <c r="O17" s="11" t="s">
         <v>26</v>
       </c>
@@ -1372,7 +1394,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="8">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="8" t="s">
@@ -1385,15 +1407,13 @@
         <v>-50</v>
       </c>
       <c r="H18" s="21">
-        <f t="shared" si="0"/>
-        <v>-0.87266388888888891</v>
+        <v>-0.85</v>
       </c>
       <c r="I18" s="5">
         <v>50</v>
       </c>
       <c r="J18" s="21">
-        <f t="shared" si="1"/>
-        <v>0.87266388888888891</v>
+        <v>0.85</v>
       </c>
       <c r="K18" s="20">
         <v>8192</v>
@@ -1402,9 +1422,11 @@
         <v>6000</v>
       </c>
       <c r="M18" s="5">
-        <v>8892</v>
-      </c>
-      <c r="N18" s="5"/>
+        <v>8890</v>
+      </c>
+      <c r="N18" s="5">
+        <v>1110822</v>
+      </c>
       <c r="O18" s="11" t="s">
         <v>27</v>
       </c>
@@ -1422,7 +1444,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="8">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>23</v>
@@ -1437,15 +1459,13 @@
         <v>-10</v>
       </c>
       <c r="H19" s="21">
-        <f t="shared" si="0"/>
-        <v>-0.17453277777777779</v>
+        <v>-0.15</v>
       </c>
       <c r="I19" s="5">
         <v>110</v>
       </c>
       <c r="J19" s="21">
-        <f t="shared" si="1"/>
-        <v>1.9198605555555555</v>
+        <v>1.85</v>
       </c>
       <c r="K19" s="20">
         <v>81920</v>
@@ -1454,9 +1474,11 @@
         <v>8000</v>
       </c>
       <c r="M19" s="5">
-        <v>5493</v>
-      </c>
-      <c r="N19" s="5"/>
+        <v>5495</v>
+      </c>
+      <c r="N19" s="5">
+        <v>1195569</v>
+      </c>
       <c r="O19" s="11" t="s">
         <v>27</v>
       </c>
@@ -1474,7 +1496,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>23</v>
@@ -1496,8 +1518,7 @@
         <v>50</v>
       </c>
       <c r="J20" s="21">
-        <f t="shared" si="1"/>
-        <v>0.87266388888888891</v>
+        <v>0.8</v>
       </c>
       <c r="K20" s="20">
         <v>8192</v>
@@ -1508,7 +1529,9 @@
       <c r="M20" s="5">
         <v>6228</v>
       </c>
-      <c r="N20" s="5"/>
+      <c r="N20" s="5">
+        <v>1159284</v>
+      </c>
       <c r="O20" s="11" t="s">
         <v>26</v>
       </c>
@@ -1526,7 +1549,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="8">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="8" t="s">
@@ -1558,7 +1581,9 @@
       <c r="M21" s="5">
         <v>10238</v>
       </c>
-      <c r="N21" s="5"/>
+      <c r="N21" s="5">
+        <v>1079648</v>
+      </c>
       <c r="O21" s="11" t="s">
         <v>26</v>
       </c>
@@ -1628,7 +1653,7 @@
         <v>98596</v>
       </c>
       <c r="D28" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>43</v>
@@ -1660,7 +1685,7 @@
         <v>98593</v>
       </c>
       <c r="D29" s="5">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>44</v>
@@ -1672,7 +1697,7 @@
         <v>27</v>
       </c>
       <c r="J29" s="10">
-        <v>5.9999999999999995E-4</v>
+        <v>0.02</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -1750,6 +1775,22 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
+    <row r="37" spans="5:8">
+      <c r="G37" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H37" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="38" spans="5:8">
+      <c r="G38" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>
@@ -1758,10 +1799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:P31"/>
+  <dimension ref="A3:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:N6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1907,7 +1948,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>23</v>
@@ -1922,15 +1963,13 @@
         <v>-80</v>
       </c>
       <c r="H8" s="21">
-        <f>G8 * 200000 * 3.14159 / (360 * 100000)</f>
-        <v>-1.3962622222222223</v>
+        <v>-1.3</v>
       </c>
       <c r="I8" s="5">
         <v>80</v>
       </c>
       <c r="J8" s="21">
-        <f>I8 * 200000 * 3.14159 / (360 * 100000)</f>
-        <v>1.3962622222222223</v>
+        <v>1.3</v>
       </c>
       <c r="K8" s="20">
         <v>8192</v>
@@ -1939,10 +1978,10 @@
         <v>12000</v>
       </c>
       <c r="M8" s="5">
-        <v>8110</v>
+        <v>8106</v>
       </c>
       <c r="N8" s="5">
-        <v>1182049</v>
+        <v>1169493</v>
       </c>
       <c r="O8" s="11" t="s">
         <v>27</v>
@@ -1959,7 +1998,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>23</v>
@@ -1974,7 +2013,7 @@
         <v>-195</v>
       </c>
       <c r="H9" s="21">
-        <f t="shared" ref="H9:H16" si="0">G9 * 200000 * 3.14159 / (360 * 100000)</f>
+        <f t="shared" ref="H9:H14" si="0">G9 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>-3.4033891666666665</v>
       </c>
       <c r="I9" s="5">
@@ -2011,7 +2050,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="8">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>23</v>
@@ -2033,8 +2072,7 @@
         <v>108</v>
       </c>
       <c r="J10" s="21">
-        <f t="shared" si="1"/>
-        <v>1.884954</v>
+        <v>1.8</v>
       </c>
       <c r="K10" s="20">
         <v>8192</v>
@@ -2063,7 +2101,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="8">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="8" t="s">
@@ -2076,15 +2114,13 @@
         <v>-90</v>
       </c>
       <c r="H11" s="21">
-        <f t="shared" si="0"/>
-        <v>-1.5707949999999999</v>
+        <v>-1.5</v>
       </c>
       <c r="I11" s="5">
         <v>90</v>
       </c>
       <c r="J11" s="21">
-        <f t="shared" si="1"/>
-        <v>1.5707949999999999</v>
+        <v>1.5</v>
       </c>
       <c r="K11" s="20">
         <v>8192</v>
@@ -2093,10 +2129,10 @@
         <v>0</v>
       </c>
       <c r="M11" s="5">
-        <v>9581</v>
+        <v>9578</v>
       </c>
       <c r="N11" s="5">
-        <v>1204800</v>
+        <v>1195569</v>
       </c>
       <c r="O11" s="11" t="s">
         <v>26</v>
@@ -2113,7 +2149,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="8">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>23</v>
@@ -2128,27 +2164,26 @@
         <v>-135</v>
       </c>
       <c r="H12" s="21">
-        <f t="shared" si="0"/>
-        <v>-2.3561925000000001</v>
+        <v>-2.2999999999999998</v>
       </c>
       <c r="I12" s="5">
-        <v>0</v>
+        <v>-1.1479999999999999</v>
       </c>
       <c r="J12" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2.0036362888888885E-2</v>
       </c>
       <c r="K12" s="20">
         <v>8192</v>
       </c>
       <c r="L12" s="5">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="M12" s="5">
-        <v>13556</v>
+        <v>11270</v>
       </c>
       <c r="N12" s="5">
-        <v>1307200</v>
+        <v>1299873</v>
       </c>
       <c r="O12" s="11" t="s">
         <v>27</v>
@@ -2165,7 +2200,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>23</v>
@@ -2180,15 +2215,13 @@
         <v>-195</v>
       </c>
       <c r="H13" s="21">
-        <f t="shared" si="0"/>
-        <v>-3.4033891666666665</v>
+        <v>-3.3</v>
       </c>
       <c r="I13" s="5">
         <v>95</v>
       </c>
       <c r="J13" s="21">
-        <f t="shared" si="1"/>
-        <v>1.6580613888888889</v>
+        <v>1.6</v>
       </c>
       <c r="K13" s="20">
         <v>81920</v>
@@ -2197,10 +2230,10 @@
         <v>11000</v>
       </c>
       <c r="M13" s="5">
-        <v>10893</v>
+        <v>10894</v>
       </c>
       <c r="N13" s="5">
-        <v>5437344</v>
+        <v>5302531</v>
       </c>
       <c r="O13" s="11" t="s">
         <v>27</v>
@@ -2217,7 +2250,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="8">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>23</v>
@@ -2239,8 +2272,7 @@
         <v>30</v>
       </c>
       <c r="J14" s="21">
-        <f t="shared" si="1"/>
-        <v>0.52359833333333339</v>
+        <v>0.5</v>
       </c>
       <c r="K14" s="20">
         <v>81920</v>
@@ -2269,7 +2301,7 @@
         <v>22</v>
       </c>
       <c r="C15" s="8">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="8" t="s">
@@ -2282,15 +2314,13 @@
         <v>-90</v>
       </c>
       <c r="H15" s="21">
-        <f t="shared" si="0"/>
-        <v>-1.5707949999999999</v>
+        <v>-1.5</v>
       </c>
       <c r="I15" s="5">
         <v>90</v>
       </c>
       <c r="J15" s="21">
-        <f t="shared" si="1"/>
-        <v>1.5707949999999999</v>
+        <v>1.5</v>
       </c>
       <c r="K15" s="20">
         <v>8192</v>
@@ -2299,10 +2329,10 @@
         <v>6000</v>
       </c>
       <c r="M15" s="5">
-        <v>8364</v>
+        <v>8346</v>
       </c>
       <c r="N15" s="5">
-        <v>1204800</v>
+        <v>1195569</v>
       </c>
       <c r="O15" s="11" t="s">
         <v>26</v>
@@ -2319,7 +2349,7 @@
         <v>23</v>
       </c>
       <c r="C16" s="8">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>23</v>
@@ -2334,8 +2364,7 @@
         <v>-135</v>
       </c>
       <c r="H16" s="21">
-        <f t="shared" si="0"/>
-        <v>-2.3561925000000001</v>
+        <v>-2.2999999999999998</v>
       </c>
       <c r="I16" s="5">
         <v>0</v>
@@ -2345,16 +2374,16 @@
         <v>0</v>
       </c>
       <c r="K16" s="20">
-        <v>81920</v>
+        <v>8192</v>
       </c>
       <c r="L16" s="5">
         <v>0</v>
       </c>
       <c r="M16" s="5">
-        <v>12707</v>
+        <v>12663</v>
       </c>
       <c r="N16" s="5">
-        <v>4072007</v>
+        <v>1299873</v>
       </c>
       <c r="O16" s="11" t="s">
         <v>26</v>
@@ -2444,7 +2473,7 @@
         <v>27</v>
       </c>
       <c r="J25" s="10">
-        <v>5.9999999999999995E-4</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -2501,6 +2530,22 @@
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
+    </row>
+    <row r="33" spans="7:8">
+      <c r="G33" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H33" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8">
+      <c r="G34" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2509,10 +2554,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:P30"/>
+  <dimension ref="A3:P33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2611,7 +2656,7 @@
         <v>26</v>
       </c>
       <c r="C8" s="8">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="8" t="s">
@@ -2624,15 +2669,13 @@
         <v>-90</v>
       </c>
       <c r="H8" s="21">
-        <f>G8 * 200000 * 3.14159 / (360 * 100000)</f>
-        <v>-1.5707949999999999</v>
+        <v>-1.5</v>
       </c>
       <c r="I8" s="5">
         <v>90</v>
       </c>
       <c r="J8" s="21">
-        <f>I8 * 200000 * 3.14159 / (360 * 100000)</f>
-        <v>1.5707949999999999</v>
+        <v>1.5</v>
       </c>
       <c r="K8" s="20">
         <v>8192</v>
@@ -2644,7 +2687,7 @@
         <v>7994</v>
       </c>
       <c r="N8" s="5">
-        <v>1204800</v>
+        <v>1195569</v>
       </c>
       <c r="O8" s="11" t="s">
         <v>26</v>
@@ -2661,7 +2704,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="8">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="8" t="s">
@@ -2674,15 +2717,13 @@
         <v>-30</v>
       </c>
       <c r="H9" s="21">
-        <f t="shared" ref="H9:H13" si="0">G9 * 200000 * 3.14159 / (360 * 100000)</f>
-        <v>-0.52359833333333339</v>
+        <v>-0.48</v>
       </c>
       <c r="I9" s="5">
         <v>30</v>
       </c>
       <c r="J9" s="21">
-        <f t="shared" ref="J9:J13" si="1">I9 * 200000 * 3.14159 / (360 * 100000)</f>
-        <v>0.52359833333333339</v>
+        <v>0.48</v>
       </c>
       <c r="K9" s="20">
         <v>8192</v>
@@ -2691,10 +2732,10 @@
         <v>0</v>
       </c>
       <c r="M9" s="5">
-        <v>11669</v>
+        <v>11640</v>
       </c>
       <c r="N9" s="5">
-        <v>1068266</v>
+        <v>1062582</v>
       </c>
       <c r="O9" s="11" t="s">
         <v>27</v>
@@ -2711,7 +2752,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="8">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
@@ -2724,15 +2765,13 @@
         <v>-80</v>
       </c>
       <c r="H10" s="21">
-        <f t="shared" si="0"/>
-        <v>-1.3962622222222223</v>
+        <v>-0.69</v>
       </c>
       <c r="I10" s="5">
         <v>45</v>
       </c>
       <c r="J10" s="21">
-        <f t="shared" si="1"/>
-        <v>0.78539749999999997</v>
+        <v>0.8</v>
       </c>
       <c r="K10" s="20">
         <v>8192</v>
@@ -2741,10 +2780,10 @@
         <v>0</v>
       </c>
       <c r="M10" s="5">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="N10" s="5">
-        <v>1182049</v>
+        <v>1089962</v>
       </c>
       <c r="O10" s="11" t="s">
         <v>27</v>
@@ -2761,7 +2800,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="8">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="8" t="s">
@@ -2774,15 +2813,13 @@
         <v>-90</v>
       </c>
       <c r="H11" s="21">
-        <f t="shared" si="0"/>
-        <v>-1.5707949999999999</v>
+        <v>-1.5</v>
       </c>
       <c r="I11" s="5">
         <v>90</v>
       </c>
       <c r="J11" s="21">
-        <f t="shared" si="1"/>
-        <v>1.5707949999999999</v>
+        <v>1.5</v>
       </c>
       <c r="K11" s="20">
         <v>8192</v>
@@ -2791,10 +2828,10 @@
         <v>10000</v>
       </c>
       <c r="M11" s="5">
-        <v>8195</v>
+        <v>8321</v>
       </c>
       <c r="N11" s="5">
-        <v>1204800</v>
+        <v>1195569</v>
       </c>
       <c r="O11" s="11" t="s">
         <v>27</v>
@@ -2811,7 +2848,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="8">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="8" t="s">
@@ -2824,15 +2861,13 @@
         <v>-30</v>
       </c>
       <c r="H12" s="21">
-        <f t="shared" si="0"/>
-        <v>-0.52359833333333339</v>
+        <v>-0.48</v>
       </c>
       <c r="I12" s="5">
         <v>30</v>
       </c>
       <c r="J12" s="21">
-        <f t="shared" si="1"/>
-        <v>0.52359833333333339</v>
+        <v>0.48</v>
       </c>
       <c r="K12" s="20">
         <v>8192</v>
@@ -2841,10 +2876,10 @@
         <v>0</v>
       </c>
       <c r="M12" s="5">
-        <v>5756</v>
+        <v>5777</v>
       </c>
       <c r="N12" s="5">
-        <v>1068266</v>
+        <v>1062582</v>
       </c>
       <c r="O12" s="11" t="s">
         <v>26</v>
@@ -2861,7 +2896,7 @@
         <v>31</v>
       </c>
       <c r="C13" s="8">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="8" t="s">
@@ -2874,15 +2909,13 @@
         <v>-45</v>
       </c>
       <c r="H13" s="21">
-        <f t="shared" si="0"/>
-        <v>-0.78539749999999997</v>
+        <v>-0.9</v>
       </c>
       <c r="I13" s="5">
         <v>80</v>
       </c>
       <c r="J13" s="21">
-        <f t="shared" si="1"/>
-        <v>1.3962622222222223</v>
+        <v>0.7</v>
       </c>
       <c r="K13" s="20">
         <v>8192</v>
@@ -2891,10 +2924,10 @@
         <v>0</v>
       </c>
       <c r="M13" s="5">
-        <v>10748</v>
+        <v>10742</v>
       </c>
       <c r="N13" s="5">
-        <v>1102400</v>
+        <v>1117341</v>
       </c>
       <c r="O13" s="11" t="s">
         <v>26</v>
@@ -2984,7 +3017,7 @@
         <v>98579</v>
       </c>
       <c r="D23" s="5">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -3012,7 +3045,7 @@
         <v>98571</v>
       </c>
       <c r="D24" s="5">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -3026,7 +3059,7 @@
         <v>27</v>
       </c>
       <c r="J24" s="10">
-        <v>5.9999999999999995E-4</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -3119,6 +3152,22 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
+    <row r="32" spans="1:10">
+      <c r="G32" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H32" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8">
+      <c r="G33" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add coman robot_ids_test_pos_deg zmq_pub walkman base_port 9500
</commit_message>
<xml_diff>
--- a/configs/Disney Coman motor parameters.xlsx
+++ b/configs/Disney Coman motor parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Legs" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="104">
   <si>
     <t>Disney Legs</t>
   </si>
@@ -73,6 +73,9 @@
     <t>Pitch</t>
   </si>
   <si>
+    <t>waist_p</t>
+  </si>
+  <si>
     <t>*</t>
   </si>
   <si>
@@ -88,6 +91,9 @@
     <t>Roll</t>
   </si>
   <si>
+    <t>waist_r</t>
+  </si>
+  <si>
     <t>0x1023</t>
   </si>
   <si>
@@ -100,49 +106,85 @@
     <t>R hip</t>
   </si>
   <si>
+    <t>RL_H_P</t>
+  </si>
+  <si>
     <t>0x2012</t>
   </si>
   <si>
     <t>L hip</t>
   </si>
   <si>
+    <t>LL_H_P</t>
+  </si>
+  <si>
     <t>0x2023</t>
   </si>
   <si>
     <t>R leg side-side</t>
   </si>
   <si>
+    <t>RL_H_R</t>
+  </si>
+  <si>
     <t>R thigh rotate</t>
   </si>
   <si>
+    <t>RL_H_Y</t>
+  </si>
+  <si>
     <t>0x1012</t>
   </si>
   <si>
     <t>R knee</t>
   </si>
   <si>
+    <t>RL_K</t>
+  </si>
+  <si>
     <t>R toe lift</t>
   </si>
   <si>
+    <t>RL_A_P</t>
+  </si>
+  <si>
     <t>R foot side-side</t>
   </si>
   <si>
+    <t>RL_A_R</t>
+  </si>
+  <si>
     <t>L leg side-side</t>
   </si>
   <si>
+    <t>LL_H_R</t>
+  </si>
+  <si>
     <t>L thigh rotate</t>
   </si>
   <si>
+    <t>LL_H_Y</t>
+  </si>
+  <si>
     <t>L knee</t>
   </si>
   <si>
+    <t>LL_K</t>
+  </si>
+  <si>
     <t>0x2033</t>
   </si>
   <si>
     <t>L toe lift</t>
   </si>
   <si>
+    <t>LL_A_P</t>
+  </si>
+  <si>
     <t>L foot side-side</t>
+  </si>
+  <si>
+    <t>LL_A_R</t>
   </si>
   <si>
     <t>FT Sensors</t>
@@ -423,7 +465,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -441,10 +483,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -510,10 +548,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -605,32 +639,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:R38"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H41" activeCellId="0" sqref="H41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.004048582996"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.2834008097166"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.7125506072875"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="16.1376518218624"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.5668016194332"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.4251012145749"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="16.004048582996"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="1" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.1417004048583"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.2834008097166"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.7125506072875"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="16.1376518218624"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.5668016194332"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.4251012145749"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0"/>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
@@ -644,13 +678,31 @@
       <c r="K1" s="0"/>
       <c r="L1" s="0"/>
       <c r="M1" s="0"/>
-      <c r="P1" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N1" s="0"/>
+      <c r="Q1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0"/>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="Q2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="0"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="0"/>
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
@@ -662,9 +714,10 @@
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
-      <c r="P3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N3" s="0"/>
+      <c r="Q3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="0"/>
       <c r="C4" s="0"/>
@@ -678,808 +731,870 @@
       <c r="K4" s="0"/>
       <c r="L4" s="0"/>
       <c r="M4" s="0"/>
-      <c r="P4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="Q4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
+      <c r="Q5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="P6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="Q6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="5"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="4"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="11"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="4" t="n">
+      <c r="D8" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="3" t="n">
+      <c r="G8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="3" t="n">
         <v>-20</v>
       </c>
-      <c r="H8" s="12" t="n">
-        <f aca="false">G8 * 200000 * 3.14159 / (360 * 100000)</f>
+      <c r="I8" s="11" t="n">
+        <f aca="false">H8 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>-0.349065555555556</v>
       </c>
-      <c r="I8" s="3" t="n">
+      <c r="J8" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="J8" s="12" t="n">
+      <c r="K8" s="11" t="n">
         <v>0.85</v>
       </c>
-      <c r="K8" s="13" t="n">
+      <c r="L8" s="12" t="n">
         <v>81920</v>
       </c>
-      <c r="L8" s="3" t="n">
+      <c r="M8" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M8" s="3" t="n">
+      <c r="N8" s="3" t="n">
         <v>11693</v>
       </c>
-      <c r="N8" s="3" t="n">
+      <c r="O8" s="3" t="n">
         <v>1455116</v>
       </c>
-      <c r="O8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P8" s="15" t="n">
+      <c r="P8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="14" t="n">
         <v>-1.383</v>
       </c>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="17"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="4" t="n">
+      <c r="D9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="3" t="n">
         <v>-30</v>
       </c>
-      <c r="H9" s="12" t="n">
+      <c r="I9" s="11" t="n">
         <v>-0.5</v>
       </c>
-      <c r="I9" s="3" t="n">
+      <c r="J9" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="J9" s="12" t="n">
+      <c r="K9" s="11" t="n">
         <v>0.5</v>
       </c>
-      <c r="K9" s="13" t="n">
+      <c r="L9" s="12" t="n">
         <v>8192</v>
       </c>
-      <c r="L9" s="3" t="n">
+      <c r="M9" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M9" s="3" t="n">
+      <c r="N9" s="3" t="n">
         <v>5342</v>
       </c>
-      <c r="N9" s="3" t="n">
+      <c r="O9" s="3" t="n">
         <v>1065189</v>
       </c>
-      <c r="O9" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" s="15" t="n">
+      <c r="P9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" s="14" t="n">
         <v>1.926</v>
       </c>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="17"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="n">
+      <c r="D10" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>27</v>
+      <c r="E10" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="3" t="n">
         <v>-110</v>
       </c>
-      <c r="H10" s="12" t="n">
-        <f aca="false">G10 * 200000 * 3.14159 / (360 * 100000)</f>
+      <c r="I10" s="11" t="n">
+        <f aca="false">H10 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>-1.91986055555556</v>
       </c>
-      <c r="I10" s="3" t="n">
+      <c r="J10" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="J10" s="12" t="n">
-        <f aca="false">I10 * 200000 * 3.14159 / (360 * 100000)</f>
+      <c r="K10" s="11" t="n">
+        <f aca="false">J10 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>0.7853975</v>
       </c>
-      <c r="K10" s="13" t="n">
+      <c r="L10" s="12" t="n">
         <v>81920</v>
       </c>
-      <c r="L10" s="3" t="n">
+      <c r="M10" s="3" t="n">
         <v>14000</v>
       </c>
-      <c r="M10" s="3" t="n">
+      <c r="N10" s="3" t="n">
         <v>8430</v>
       </c>
-      <c r="N10" s="3" t="n">
+      <c r="O10" s="3" t="n">
         <v>3503108</v>
       </c>
-      <c r="O10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P10" s="15" t="n">
+      <c r="P10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" s="14" t="n">
         <v>-2.529</v>
       </c>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="17"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="4" t="n">
+      <c r="D11" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>29</v>
+      <c r="E11" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="3" t="n">
         <v>-110</v>
       </c>
-      <c r="H11" s="12" t="n">
+      <c r="I11" s="11" t="n">
         <v>-1.9</v>
       </c>
-      <c r="I11" s="3" t="n">
+      <c r="J11" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="J11" s="12" t="n">
-        <f aca="false">I11 * 200000 * 3.14159 / (360 * 100000)</f>
+      <c r="K11" s="11" t="n">
+        <f aca="false">J11 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>0.7853975</v>
       </c>
-      <c r="K11" s="13" t="n">
+      <c r="L11" s="12" t="n">
         <v>81920</v>
       </c>
-      <c r="L11" s="3" t="n">
+      <c r="M11" s="3" t="n">
         <v>3000</v>
       </c>
-      <c r="M11" s="3" t="n">
+      <c r="N11" s="3" t="n">
         <v>9626</v>
       </c>
-      <c r="N11" s="3" t="n">
+      <c r="O11" s="3" t="n">
         <v>3477214</v>
       </c>
-      <c r="O11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P11" s="15" t="n">
+      <c r="P11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" s="14" t="n">
         <v>2.514</v>
       </c>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="17"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="4" t="n">
+      <c r="D12" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="E12" s="3"/>
       <c r="F12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="3" t="n">
         <v>-60</v>
       </c>
-      <c r="H12" s="12" t="n">
+      <c r="I12" s="11" t="n">
         <v>-1</v>
       </c>
-      <c r="I12" s="3" t="n">
+      <c r="J12" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="J12" s="12" t="n">
-        <f aca="false">I12 * 200000 * 3.14159 / (360 * 100000)</f>
+      <c r="K12" s="11" t="n">
+        <f aca="false">J12 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>0.436331944444444</v>
       </c>
-      <c r="K12" s="13" t="n">
+      <c r="L12" s="12" t="n">
         <v>8192</v>
       </c>
-      <c r="L12" s="3" t="n">
+      <c r="M12" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M12" s="3" t="n">
+      <c r="N12" s="3" t="n">
         <v>7394</v>
       </c>
-      <c r="N12" s="3" t="n">
+      <c r="O12" s="3" t="n">
         <v>1130379</v>
       </c>
-      <c r="O12" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12" s="15" t="n">
+      <c r="P12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" s="14" t="n">
         <v>1.668</v>
       </c>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="17"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="4" t="n">
+      <c r="D13" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="E13" s="3"/>
       <c r="F13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="3" t="n">
         <v>-50</v>
       </c>
-      <c r="H13" s="12" t="n">
-        <f aca="false">G13 * 200000 * 3.14159 / (360 * 100000)</f>
+      <c r="I13" s="11" t="n">
+        <f aca="false">H13 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>-0.872663888888889</v>
       </c>
-      <c r="I13" s="3" t="n">
+      <c r="J13" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="J13" s="12" t="n">
+      <c r="K13" s="11" t="n">
         <v>0.86</v>
       </c>
-      <c r="K13" s="13" t="n">
+      <c r="L13" s="12" t="n">
         <v>8192</v>
       </c>
-      <c r="L13" s="3" t="n">
+      <c r="M13" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M13" s="3" t="n">
+      <c r="N13" s="3" t="n">
         <v>4894</v>
       </c>
-      <c r="N13" s="3" t="n">
+      <c r="O13" s="3" t="n">
         <v>1113782</v>
       </c>
-      <c r="O13" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P13" s="15" t="n">
+      <c r="P13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13" s="14" t="n">
         <v>-1.647</v>
       </c>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="17"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="4" t="n">
+      <c r="D14" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="3" t="n">
+      <c r="G14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="3" t="n">
         <v>-10</v>
       </c>
-      <c r="H14" s="12" t="n">
-        <f aca="false">G14 * 200000 * 3.14159 / (360 * 100000)</f>
+      <c r="I14" s="11" t="n">
+        <f aca="false">H14 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>-0.174532777777778</v>
       </c>
-      <c r="I14" s="3" t="n">
+      <c r="J14" s="3" t="n">
         <v>110</v>
       </c>
-      <c r="J14" s="12" t="n">
+      <c r="K14" s="11" t="n">
         <v>1.88</v>
       </c>
-      <c r="K14" s="13" t="n">
+      <c r="L14" s="12" t="n">
         <v>81920</v>
       </c>
-      <c r="L14" s="3" t="n">
+      <c r="M14" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M14" s="3" t="n">
+      <c r="N14" s="3" t="n">
         <v>8413</v>
       </c>
-      <c r="N14" s="3" t="n">
+      <c r="O14" s="3" t="n">
         <v>1227551</v>
       </c>
-      <c r="O14" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P14" s="15" t="n">
+      <c r="P14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q14" s="14" t="n">
         <v>-1.653</v>
       </c>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="17"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C15" s="4" t="n">
+      <c r="D15" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="3" t="n">
+      <c r="G15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="3" t="n">
         <v>-70</v>
       </c>
-      <c r="H15" s="12" t="n">
+      <c r="I15" s="11" t="n">
         <v>-1.2</v>
       </c>
-      <c r="I15" s="3" t="n">
+      <c r="J15" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="J15" s="12" t="n">
-        <f aca="false">I15 * 200000 * 3.14159 / (360 * 100000)</f>
+      <c r="K15" s="11" t="n">
+        <f aca="false">J15 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>0.872663888888889</v>
       </c>
-      <c r="K15" s="13" t="n">
+      <c r="L15" s="12" t="n">
         <v>8192</v>
       </c>
-      <c r="L15" s="3" t="n">
+      <c r="M15" s="3" t="n">
         <v>8000</v>
       </c>
-      <c r="M15" s="3" t="n">
+      <c r="N15" s="3" t="n">
         <v>7924</v>
       </c>
-      <c r="N15" s="3" t="n">
+      <c r="O15" s="3" t="n">
         <v>1156455</v>
       </c>
-      <c r="O15" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P15" s="15" t="n">
+      <c r="P15" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="14" t="n">
         <v>-2.121</v>
       </c>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="17"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="16"/>
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>-35</v>
+      </c>
+      <c r="I16" s="11" t="n">
+        <f aca="false">H16 * 200000 * 3.14159 / (360 * 100000)</f>
+        <v>-0.610864722222222</v>
+      </c>
+      <c r="J16" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="B16" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="n">
-        <v>13</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="3" t="n">
-        <v>-35</v>
-      </c>
-      <c r="H16" s="12" t="n">
-        <f aca="false">G16 * 200000 * 3.14159 / (360 * 100000)</f>
-        <v>-0.610864722222222</v>
-      </c>
-      <c r="I16" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="J16" s="12" t="n">
-        <f aca="false">I16 * 200000 * 3.14159 / (360 * 100000)</f>
+      <c r="K16" s="11" t="n">
+        <f aca="false">J16 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>0.610864722222222</v>
       </c>
-      <c r="K16" s="13" t="n">
+      <c r="L16" s="12" t="n">
         <v>8192</v>
       </c>
-      <c r="L16" s="3" t="n">
+      <c r="M16" s="3" t="n">
         <v>4000</v>
       </c>
-      <c r="M16" s="3" t="n">
+      <c r="N16" s="3" t="n">
         <v>8949</v>
       </c>
-      <c r="N16" s="3" t="n">
+      <c r="O16" s="3" t="n">
         <v>1079648</v>
       </c>
-      <c r="O16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P16" s="15" t="n">
+      <c r="P16" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q16" s="14" t="n">
         <v>2.31</v>
       </c>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="17"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="16"/>
     </row>
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="C17" s="4" t="n">
+      <c r="D17" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="E17" s="3"/>
       <c r="F17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="3" t="n">
         <v>-25</v>
       </c>
-      <c r="H17" s="12" t="n">
+      <c r="I17" s="11" t="n">
         <v>-0.4</v>
       </c>
-      <c r="I17" s="3" t="n">
+      <c r="J17" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="J17" s="12" t="n">
+      <c r="K17" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="K17" s="13" t="n">
+      <c r="L17" s="12" t="n">
         <v>8192</v>
       </c>
-      <c r="L17" s="3" t="n">
+      <c r="M17" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M17" s="3" t="n">
+      <c r="N17" s="3" t="n">
         <v>1189</v>
       </c>
-      <c r="N17" s="3" t="n">
+      <c r="O17" s="3" t="n">
         <v>1052151</v>
       </c>
-      <c r="O17" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P17" s="15" t="n">
+      <c r="P17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q17" s="14" t="n">
         <v>1.571</v>
       </c>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="17"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="C18" s="4" t="n">
+      <c r="D18" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="E18" s="3"/>
       <c r="F18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="3" t="n">
         <v>-50</v>
       </c>
-      <c r="H18" s="12" t="n">
+      <c r="I18" s="11" t="n">
         <v>-0.85</v>
       </c>
-      <c r="I18" s="3" t="n">
+      <c r="J18" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="J18" s="12" t="n">
+      <c r="K18" s="11" t="n">
         <v>0.85</v>
       </c>
-      <c r="K18" s="13" t="n">
+      <c r="L18" s="12" t="n">
         <v>8192</v>
       </c>
-      <c r="L18" s="3" t="n">
+      <c r="M18" s="3" t="n">
         <v>6000</v>
       </c>
-      <c r="M18" s="3" t="n">
+      <c r="N18" s="3" t="n">
         <v>8890</v>
       </c>
-      <c r="N18" s="3" t="n">
+      <c r="O18" s="3" t="n">
         <v>1110822</v>
       </c>
-      <c r="O18" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P18" s="15" t="n">
+      <c r="P18" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q18" s="14" t="n">
         <v>-2.85</v>
       </c>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="17"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="16"/>
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="3" t="n">
+        <v>49</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="C19" s="4" t="n">
+      <c r="D19" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>39</v>
+      <c r="E19" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="3" t="n">
+        <v>51</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="3" t="n">
         <v>-10</v>
       </c>
-      <c r="H19" s="12" t="n">
+      <c r="I19" s="11" t="n">
         <v>-0.15</v>
       </c>
-      <c r="I19" s="3" t="n">
+      <c r="J19" s="3" t="n">
         <v>110</v>
       </c>
-      <c r="J19" s="12" t="n">
+      <c r="K19" s="11" t="n">
         <v>1.85</v>
       </c>
-      <c r="K19" s="13" t="n">
+      <c r="L19" s="12" t="n">
         <v>81920</v>
       </c>
-      <c r="L19" s="3" t="n">
+      <c r="M19" s="3" t="n">
         <v>8000</v>
       </c>
-      <c r="M19" s="3" t="n">
+      <c r="N19" s="3" t="n">
         <v>5495</v>
       </c>
-      <c r="N19" s="3" t="n">
+      <c r="O19" s="3" t="n">
         <v>1195569</v>
       </c>
-      <c r="O19" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P19" s="15" t="n">
+      <c r="P19" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q19" s="14" t="n">
         <v>-2.208</v>
       </c>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="17"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="3" t="n">
+        <v>52</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="C20" s="4" t="n">
+      <c r="D20" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>39</v>
+      <c r="E20" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="3" t="n">
+        <v>51</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="3" t="n">
         <v>-70</v>
       </c>
-      <c r="H20" s="12" t="n">
-        <f aca="false">G20 * 200000 * 3.14159 / (360 * 100000)</f>
+      <c r="I20" s="11" t="n">
+        <f aca="false">H20 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>-1.22172944444444</v>
       </c>
-      <c r="I20" s="3" t="n">
+      <c r="J20" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="J20" s="12" t="n">
+      <c r="K20" s="11" t="n">
         <v>0.8</v>
       </c>
-      <c r="K20" s="13" t="n">
+      <c r="L20" s="12" t="n">
         <v>8192</v>
       </c>
-      <c r="L20" s="3" t="n">
+      <c r="M20" s="3" t="n">
         <v>8000</v>
       </c>
-      <c r="M20" s="3" t="n">
+      <c r="N20" s="3" t="n">
         <v>6228</v>
       </c>
-      <c r="N20" s="3" t="n">
+      <c r="O20" s="3" t="n">
         <v>1159284</v>
       </c>
-      <c r="O20" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P20" s="15" t="n">
+      <c r="P20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q20" s="14" t="n">
         <v>2.544</v>
       </c>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="17"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="16"/>
     </row>
     <row r="21" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="3" t="n">
+        <v>54</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C21" s="4" t="n">
+      <c r="D21" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="E21" s="3"/>
       <c r="F21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="3" t="n">
         <v>-35</v>
       </c>
-      <c r="H21" s="12" t="n">
-        <f aca="false">G21 * 200000 * 3.14159 / (360 * 100000)</f>
+      <c r="I21" s="11" t="n">
+        <f aca="false">H21 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>-0.610864722222222</v>
       </c>
-      <c r="I21" s="3" t="n">
+      <c r="J21" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="J21" s="12" t="n">
-        <f aca="false">I21 * 200000 * 3.14159 / (360 * 100000)</f>
+      <c r="K21" s="11" t="n">
+        <f aca="false">J21 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>0.610864722222222</v>
       </c>
-      <c r="K21" s="13" t="n">
+      <c r="L21" s="12" t="n">
         <v>8192</v>
       </c>
-      <c r="L21" s="3" t="n">
+      <c r="M21" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M21" s="3" t="n">
+      <c r="N21" s="3" t="n">
         <v>10238</v>
       </c>
-      <c r="N21" s="3" t="n">
+      <c r="O21" s="3" t="n">
         <v>1079648</v>
       </c>
-      <c r="O21" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P21" s="15" t="n">
+      <c r="P21" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q21" s="14" t="n">
         <v>2.157</v>
       </c>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="17"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R21" s="15"/>
+      <c r="S21" s="16"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
       <c r="B22" s="0"/>
       <c r="C22" s="0"/>
@@ -1493,57 +1608,61 @@
       <c r="K22" s="0"/>
       <c r="L22" s="0"/>
       <c r="M22" s="0"/>
-      <c r="P22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N22" s="0"/>
+      <c r="Q22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0"/>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
       <c r="D23" s="0"/>
       <c r="E23" s="0"/>
       <c r="F23" s="0"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="0"/>
-      <c r="P23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="0"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="0"/>
+      <c r="Q23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
       <c r="B24" s="0"/>
       <c r="C24" s="0"/>
       <c r="D24" s="0"/>
       <c r="E24" s="0"/>
       <c r="F24" s="0"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="0"/>
+      <c r="G24" s="0"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
       <c r="K24" s="0"/>
       <c r="L24" s="0"/>
       <c r="M24" s="0"/>
-      <c r="P24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N24" s="0"/>
+      <c r="Q24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
       <c r="B25" s="0"/>
       <c r="C25" s="0"/>
       <c r="D25" s="0"/>
       <c r="E25" s="0"/>
       <c r="F25" s="0"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="0"/>
+      <c r="G25" s="0"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
       <c r="K25" s="0"/>
       <c r="L25" s="0"/>
       <c r="M25" s="0"/>
-      <c r="P25" s="0"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N25" s="0"/>
+      <c r="Q25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
       <c r="B26" s="0"/>
       <c r="C26" s="0"/>
@@ -1557,206 +1676,212 @@
       <c r="K26" s="0"/>
       <c r="L26" s="0"/>
       <c r="M26" s="0"/>
-      <c r="P26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N26" s="0"/>
+      <c r="Q26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>43</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="0"/>
-      <c r="H27" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="0"/>
       <c r="I27" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-    </row>
-    <row r="28" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+    </row>
+    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="3" t="n">
+        <v>62</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="C28" s="3" t="n">
+      <c r="D28" s="3" t="n">
         <v>98596</v>
       </c>
-      <c r="D28" s="3" t="n">
+      <c r="E28" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="E28" s="0"/>
       <c r="F28" s="0"/>
-      <c r="G28" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J28" s="8" t="n">
+      <c r="G28" s="0"/>
+      <c r="H28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K28" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-    </row>
-    <row r="29" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+    </row>
+    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="3" t="n">
+        <v>66</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="D29" s="3" t="n">
         <v>98593</v>
       </c>
-      <c r="D29" s="3" t="n">
+      <c r="E29" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="E29" s="0"/>
       <c r="F29" s="0"/>
-      <c r="G29" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H29" s="8" t="n">
+      <c r="G29" s="0"/>
+      <c r="H29" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="I29" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J29" s="8" t="n">
+      <c r="J29" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="7" t="n">
         <v>0.02</v>
       </c>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
-      <c r="C30" s="0"/>
+      <c r="B30" s="0"/>
       <c r="D30" s="0"/>
       <c r="E30" s="0"/>
       <c r="F30" s="0"/>
-      <c r="G30" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-    </row>
-    <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="0"/>
+      <c r="G30" s="0"/>
+      <c r="H30" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+    </row>
+    <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
       <c r="H31" s="0"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
+      <c r="I31" s="0"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
       <c r="N31" s="10"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E32" s="0"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F32" s="0"/>
       <c r="G32" s="0"/>
       <c r="H32" s="0"/>
-      <c r="N32" s="1"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E33" s="0"/>
+      <c r="I32" s="0"/>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F33" s="0"/>
-      <c r="G33" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H33" s="1" t="n">
+      <c r="G33" s="0"/>
+      <c r="H33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I33" s="1" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E34" s="0"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F34" s="0"/>
-      <c r="G34" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="G34" s="0"/>
       <c r="H34" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E35" s="0"/>
+        <v>72</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F35" s="0"/>
-      <c r="G35" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="H35" s="1" t="n">
+      <c r="G35" s="0"/>
+      <c r="H35" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="I35" s="1" t="n">
         <v>16384</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="0"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
       <c r="H36" s="0"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G37" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="H37" s="1" t="n">
+      <c r="I36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H37" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I37" s="1" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G38" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>63</v>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H38" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1777,8 +1902,8 @@
   </sheetPr>
   <dimension ref="A3:P34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1798,7 +1923,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1859,7 +1984,7 @@
       <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1880,10 +2005,10 @@
       <c r="J6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="M6" s="3" t="s">
@@ -1892,10 +2017,10 @@
       <c r="N6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1903,23 +2028,23 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4"/>
       <c r="I7" s="3"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="5"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="9"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>1</v>
@@ -1928,27 +2053,27 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G8" s="3" t="n">
         <v>-80</v>
       </c>
-      <c r="H8" s="12" t="n">
+      <c r="H8" s="11" t="n">
         <v>-1.3</v>
       </c>
       <c r="I8" s="3" t="n">
         <v>80</v>
       </c>
-      <c r="J8" s="12" t="n">
+      <c r="J8" s="11" t="n">
         <v>1.3</v>
       </c>
-      <c r="K8" s="13" t="n">
+      <c r="K8" s="12" t="n">
         <v>8192</v>
       </c>
       <c r="L8" s="3" t="n">
@@ -1960,16 +2085,16 @@
       <c r="N8" s="3" t="n">
         <v>1169493</v>
       </c>
-      <c r="O8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P8" s="15" t="n">
+      <c r="O8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" s="14" t="n">
         <v>-1.611</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>16</v>
@@ -1978,29 +2103,29 @@
         <v>5</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G9" s="3" t="n">
         <v>-195</v>
       </c>
-      <c r="H9" s="12" t="n">
+      <c r="H9" s="11" t="n">
         <f aca="false">G9 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>-3.40338916666667</v>
       </c>
       <c r="I9" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="J9" s="12" t="n">
+      <c r="J9" s="11" t="n">
         <f aca="false">I9 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>1.65806138888889</v>
       </c>
-      <c r="K9" s="13" t="n">
+      <c r="K9" s="12" t="n">
         <v>8192</v>
       </c>
       <c r="L9" s="3" t="n">
@@ -2012,16 +2137,16 @@
       <c r="N9" s="3" t="n">
         <v>1443734</v>
       </c>
-      <c r="O9" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" s="15" t="n">
+      <c r="O9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" s="14" t="n">
         <v>1.719</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B10" s="3" t="n">
         <v>17</v>
@@ -2030,28 +2155,28 @@
         <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10" s="3" t="n">
         <v>-30</v>
       </c>
-      <c r="H10" s="12" t="n">
+      <c r="H10" s="11" t="n">
         <f aca="false">G10 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>-0.523598333333333</v>
       </c>
       <c r="I10" s="3" t="n">
         <v>108</v>
       </c>
-      <c r="J10" s="12" t="n">
+      <c r="J10" s="11" t="n">
         <v>1.8</v>
       </c>
-      <c r="K10" s="13" t="n">
+      <c r="K10" s="12" t="n">
         <v>8192</v>
       </c>
       <c r="L10" s="3" t="n">
@@ -2063,16 +2188,16 @@
       <c r="N10" s="3" t="n">
         <v>1068266</v>
       </c>
-      <c r="O10" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P10" s="15" t="n">
+      <c r="O10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" s="14" t="n">
         <v>1.875</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B11" s="3" t="n">
         <v>18</v>
@@ -2082,24 +2207,24 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G11" s="3" t="n">
         <v>-90</v>
       </c>
-      <c r="H11" s="12" t="n">
+      <c r="H11" s="11" t="n">
         <v>-1.5</v>
       </c>
       <c r="I11" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="J11" s="12" t="n">
+      <c r="J11" s="11" t="n">
         <v>1.5</v>
       </c>
-      <c r="K11" s="13" t="n">
+      <c r="K11" s="12" t="n">
         <v>8192</v>
       </c>
       <c r="L11" s="3" t="n">
@@ -2111,16 +2236,16 @@
       <c r="N11" s="3" t="n">
         <v>1195569</v>
       </c>
-      <c r="O11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P11" s="15" t="n">
+      <c r="O11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="14" t="n">
         <v>1.737</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B12" s="3" t="n">
         <v>19</v>
@@ -2129,28 +2254,28 @@
         <v>24</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G12" s="3" t="n">
         <v>-135</v>
       </c>
-      <c r="H12" s="12" t="n">
+      <c r="H12" s="11" t="n">
         <v>-2.3</v>
       </c>
       <c r="I12" s="3" t="n">
         <v>-1.148</v>
       </c>
-      <c r="J12" s="12" t="n">
+      <c r="J12" s="11" t="n">
         <f aca="false">I12 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>-0.0200363628888889</v>
       </c>
-      <c r="K12" s="13" t="n">
+      <c r="K12" s="12" t="n">
         <v>8192</v>
       </c>
       <c r="L12" s="3" t="n">
@@ -2162,16 +2287,16 @@
       <c r="N12" s="3" t="n">
         <v>1299873</v>
       </c>
-      <c r="O12" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P12" s="15" t="n">
+      <c r="O12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" s="14" t="n">
         <v>-1.758</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>20</v>
@@ -2180,27 +2305,27 @@
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G13" s="3" t="n">
         <v>-195</v>
       </c>
-      <c r="H13" s="12" t="n">
+      <c r="H13" s="11" t="n">
         <v>-3.3</v>
       </c>
       <c r="I13" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="J13" s="12" t="n">
+      <c r="J13" s="11" t="n">
         <v>1.6</v>
       </c>
-      <c r="K13" s="13" t="n">
+      <c r="K13" s="12" t="n">
         <v>81920</v>
       </c>
       <c r="L13" s="3" t="n">
@@ -2212,16 +2337,16 @@
       <c r="N13" s="3" t="n">
         <v>5302531</v>
       </c>
-      <c r="O13" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P13" s="15" t="n">
+      <c r="O13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P13" s="14" t="n">
         <v>-1.791</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="B14" s="3" t="n">
         <v>21</v>
@@ -2230,28 +2355,28 @@
         <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G14" s="3" t="n">
         <v>-108</v>
       </c>
-      <c r="H14" s="12" t="n">
+      <c r="H14" s="11" t="n">
         <f aca="false">G14 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>-1.884954</v>
       </c>
       <c r="I14" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="J14" s="12" t="n">
+      <c r="J14" s="11" t="n">
         <v>0.5</v>
       </c>
-      <c r="K14" s="13" t="n">
+      <c r="K14" s="12" t="n">
         <v>81920</v>
       </c>
       <c r="L14" s="3" t="n">
@@ -2263,16 +2388,16 @@
       <c r="N14" s="3" t="n">
         <v>3457658</v>
       </c>
-      <c r="O14" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P14" s="15" t="n">
+      <c r="O14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P14" s="14" t="n">
         <v>1.833</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B15" s="3" t="n">
         <v>22</v>
@@ -2282,24 +2407,24 @@
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G15" s="3" t="n">
         <v>-90</v>
       </c>
-      <c r="H15" s="12" t="n">
+      <c r="H15" s="11" t="n">
         <v>-1.5</v>
       </c>
       <c r="I15" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="J15" s="12" t="n">
+      <c r="J15" s="11" t="n">
         <v>1.5</v>
       </c>
-      <c r="K15" s="13" t="n">
+      <c r="K15" s="12" t="n">
         <v>8192</v>
       </c>
       <c r="L15" s="3" t="n">
@@ -2311,16 +2436,16 @@
       <c r="N15" s="3" t="n">
         <v>1195569</v>
       </c>
-      <c r="O15" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15" s="15" t="n">
+      <c r="O15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P15" s="14" t="n">
         <v>1.68</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="B16" s="3" t="n">
         <v>23</v>
@@ -2329,28 +2454,28 @@
         <v>32</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G16" s="3" t="n">
         <v>-135</v>
       </c>
-      <c r="H16" s="12" t="n">
+      <c r="H16" s="11" t="n">
         <v>-2.3</v>
       </c>
       <c r="I16" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="J16" s="12" t="n">
+      <c r="J16" s="11" t="n">
         <f aca="false">I16 * 200000 * 3.14159 / (360 * 100000)</f>
         <v>0</v>
       </c>
-      <c r="K16" s="13" t="n">
+      <c r="K16" s="12" t="n">
         <v>8192</v>
       </c>
       <c r="L16" s="3" t="n">
@@ -2362,16 +2487,16 @@
       <c r="N16" s="3" t="n">
         <v>1299873</v>
       </c>
-      <c r="O16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P16" s="15" t="n">
+      <c r="O16" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P16" s="14" t="n">
         <v>1.755</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="B17" s="3" t="n">
         <v>24</v>
@@ -2381,19 +2506,19 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="12"/>
+      <c r="H17" s="11"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="13"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="12"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="15"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="B18" s="3" t="n">
         <v>25</v>
@@ -2403,75 +2528,75 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="12"/>
+      <c r="H18" s="11"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="13"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="12"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="15"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="14"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G24" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="8" t="n">
+      <c r="G24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J24" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G25" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H25" s="8" t="n">
+      <c r="G25" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="I25" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="8" t="n">
+      <c r="I25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="7" t="n">
         <v>0.02</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G26" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>21</v>
+      <c r="G26" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="11"/>
+      <c r="J27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G28" s="1"/>
@@ -2480,7 +2605,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G29" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>100</v>
@@ -2490,17 +2615,17 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G30" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G31" s="0" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="H31" s="1" t="n">
         <v>16384</v>
@@ -2509,19 +2634,19 @@
       <c r="J31" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G33" s="24" t="s">
-        <v>61</v>
+      <c r="G33" s="22" t="s">
+        <v>75</v>
       </c>
       <c r="H33" s="1" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G34" s="24" t="s">
-        <v>62</v>
+      <c r="G34" s="22" t="s">
+        <v>76</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2542,7 +2667,7 @@
   </sheetPr>
   <dimension ref="A3:P33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -2564,7 +2689,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2577,7 +2702,7 @@
       <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -2598,10 +2723,10 @@
       <c r="J6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="M6" s="3" t="s">
@@ -2610,10 +2735,10 @@
       <c r="N6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2621,23 +2746,23 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4"/>
       <c r="I7" s="3"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="5"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="9"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>26</v>
@@ -2647,24 +2772,24 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="4" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="G8" s="3" t="n">
         <v>-90</v>
       </c>
-      <c r="H8" s="12" t="n">
+      <c r="H8" s="11" t="n">
         <v>-1.5</v>
       </c>
       <c r="I8" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="J8" s="12" t="n">
+      <c r="J8" s="11" t="n">
         <v>1.5</v>
       </c>
-      <c r="K8" s="13" t="n">
+      <c r="K8" s="12" t="n">
         <v>8192</v>
       </c>
       <c r="L8" s="3" t="n">
@@ -2676,16 +2801,16 @@
       <c r="N8" s="3" t="n">
         <v>1195569</v>
       </c>
-      <c r="O8" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="15" t="n">
+      <c r="O8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="14" t="n">
         <v>3.993</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>27</v>
@@ -2695,24 +2820,24 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="4" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="G9" s="3" t="n">
         <v>-30</v>
       </c>
-      <c r="H9" s="12" t="n">
+      <c r="H9" s="11" t="n">
         <v>-0.48</v>
       </c>
       <c r="I9" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="J9" s="12" t="n">
+      <c r="J9" s="11" t="n">
         <v>0.48</v>
       </c>
-      <c r="K9" s="13" t="n">
+      <c r="K9" s="12" t="n">
         <v>8192</v>
       </c>
       <c r="L9" s="3" t="n">
@@ -2724,16 +2849,16 @@
       <c r="N9" s="3" t="n">
         <v>1062582</v>
       </c>
-      <c r="O9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P9" s="15" t="n">
+      <c r="O9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P9" s="14" t="n">
         <v>-2.103</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="B10" s="3" t="n">
         <v>28</v>
@@ -2743,24 +2868,24 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="G10" s="3" t="n">
         <v>-80</v>
       </c>
-      <c r="H10" s="12" t="n">
+      <c r="H10" s="11" t="n">
         <v>-0.69</v>
       </c>
       <c r="I10" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="J10" s="12" t="n">
+      <c r="J10" s="11" t="n">
         <v>0.8</v>
       </c>
-      <c r="K10" s="13" t="n">
+      <c r="K10" s="12" t="n">
         <v>8192</v>
       </c>
       <c r="L10" s="3" t="n">
@@ -2772,16 +2897,16 @@
       <c r="N10" s="3" t="n">
         <v>1089962</v>
       </c>
-      <c r="O10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P10" s="15" t="n">
+      <c r="O10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P10" s="14" t="n">
         <v>-2.784</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="B11" s="3" t="n">
         <v>29</v>
@@ -2791,24 +2916,24 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="4" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="G11" s="3" t="n">
         <v>-90</v>
       </c>
-      <c r="H11" s="12" t="n">
+      <c r="H11" s="11" t="n">
         <v>-1.5</v>
       </c>
       <c r="I11" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="J11" s="12" t="n">
+      <c r="J11" s="11" t="n">
         <v>1.5</v>
       </c>
-      <c r="K11" s="13" t="n">
+      <c r="K11" s="12" t="n">
         <v>8192</v>
       </c>
       <c r="L11" s="3" t="n">
@@ -2820,16 +2945,16 @@
       <c r="N11" s="3" t="n">
         <v>1195569</v>
       </c>
-      <c r="O11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P11" s="15" t="n">
+      <c r="O11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" s="14" t="n">
         <v>-1.821</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B12" s="3" t="n">
         <v>30</v>
@@ -2839,24 +2964,24 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="4" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="G12" s="3" t="n">
         <v>-30</v>
       </c>
-      <c r="H12" s="12" t="n">
+      <c r="H12" s="11" t="n">
         <v>-0.48</v>
       </c>
       <c r="I12" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="J12" s="12" t="n">
+      <c r="J12" s="11" t="n">
         <v>0.48</v>
       </c>
-      <c r="K12" s="13" t="n">
+      <c r="K12" s="12" t="n">
         <v>8192</v>
       </c>
       <c r="L12" s="3" t="n">
@@ -2868,16 +2993,16 @@
       <c r="N12" s="3" t="n">
         <v>1062582</v>
       </c>
-      <c r="O12" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12" s="15" t="n">
+      <c r="O12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P12" s="14" t="n">
         <v>1.419</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>31</v>
@@ -2887,24 +3012,24 @@
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="G13" s="3" t="n">
         <v>-45</v>
       </c>
-      <c r="H13" s="12" t="n">
+      <c r="H13" s="11" t="n">
         <v>-0.9</v>
       </c>
       <c r="I13" s="3" t="n">
         <v>80</v>
       </c>
-      <c r="J13" s="12" t="n">
+      <c r="J13" s="11" t="n">
         <v>0.7</v>
       </c>
-      <c r="K13" s="13" t="n">
+      <c r="K13" s="12" t="n">
         <v>8192</v>
       </c>
       <c r="L13" s="3" t="n">
@@ -2916,18 +3041,18 @@
       <c r="N13" s="3" t="n">
         <v>1117341</v>
       </c>
-      <c r="O13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P13" s="15" t="n">
+      <c r="O13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="14" t="n">
         <v>4.05</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="25" t="n">
+      <c r="A14" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="23" t="n">
         <v>32</v>
       </c>
       <c r="C14" s="4"/>
@@ -2935,21 +3060,21 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="12"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="15"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="25" t="n">
+      <c r="A15" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="23" t="n">
         <v>33</v>
       </c>
       <c r="C15" s="4"/>
@@ -2957,45 +3082,45 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="12"/>
+      <c r="H15" s="11"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="15"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="14"/>
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B23" s="3" t="n">
         <v>36</v>
@@ -3008,22 +3133,22 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="8" t="n">
+      <c r="G23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J23" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="B24" s="3" t="n">
         <v>37</v>
@@ -3036,16 +3161,16 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H24" s="8" t="n">
+      <c r="G24" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I24" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J24" s="8" t="n">
+      <c r="I24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="7" t="n">
         <v>0.02</v>
       </c>
     </row>
@@ -3056,30 +3181,30 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H25" s="8" t="n">
+      <c r="G25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I25" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>21</v>
+      <c r="I25" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="21"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="11"/>
+      <c r="J26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
@@ -3100,7 +3225,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="H28" s="1" t="n">
         <v>100</v>
@@ -3116,10 +3241,10 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -3131,7 +3256,7 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="G30" s="0" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="H30" s="1" t="n">
         <v>16384</v>
@@ -3140,19 +3265,19 @@
       <c r="J30" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G32" s="24" t="s">
-        <v>61</v>
+      <c r="G32" s="22" t="s">
+        <v>75</v>
       </c>
       <c r="H32" s="1" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G33" s="24" t="s">
-        <v>62</v>
+      <c r="G33" s="22" t="s">
+        <v>76</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>